<commit_message>
changed solution to question-6
</commit_message>
<xml_diff>
--- a/Q6.xlsx
+++ b/Q6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajat/Desktop/ass-5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajat/Desktop/ass-5/-CRE--Assignmnet-5/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>K</t>
   </si>
@@ -65,15 +65,25 @@
   <si>
     <t>X(mass b)</t>
   </si>
+  <si>
+    <t>X(eb)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,14 +109,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
@@ -138,7 +166,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -574,11 +601,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="301018784"/>
-        <c:axId val="335832800"/>
+        <c:axId val="933282336"/>
+        <c:axId val="939251696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="301018784"/>
+        <c:axId val="933282336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="300.0"/>
@@ -636,12 +663,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335832800"/>
+        <c:crossAx val="939251696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335832800"/>
+        <c:axId val="939251696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,6 +688,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -697,7 +725,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301018784"/>
+        <c:crossAx val="933282336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -711,7 +739,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1458,7 +1485,7 @@
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Xeb vs T</c:v>
+            <c:v>Xe vs T</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1484,6 +1511,83 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="-0.36"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.522237985481363"/>
+                  <c:y val="0.0645416988053278"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t>y = 0.002x - 0.6809</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="2000"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet2!$B$2:$B$101</c:f>
@@ -1795,309 +1899,309 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$C$2:$C$101</c:f>
+              <c:f>Sheet2!$K$2:$K$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1218239</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1331199</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1416282</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1515006</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.156763</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1622442</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1682902</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1718953</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1758482</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.179645</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1827491</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1863982</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1885666</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1914857</c:v>
+                  <c:v>0.331215917</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1944928</c:v>
+                  <c:v>0.3796619</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1966154</c:v>
+                  <c:v>0.381076933</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.1985282</c:v>
+                  <c:v>0.382352133</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.2011171</c:v>
+                  <c:v>0.384078067</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.2027651</c:v>
+                  <c:v>0.385176717</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.2046926</c:v>
+                  <c:v>0.386461717</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.2068894</c:v>
+                  <c:v>0.38792625</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.2083315</c:v>
+                  <c:v>0.388887633</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.2100618</c:v>
+                  <c:v>0.390041217</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.211779</c:v>
+                  <c:v>0.391186</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.2132032</c:v>
+                  <c:v>0.39213545</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.2150224</c:v>
+                  <c:v>0.393348267</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.2163199</c:v>
+                  <c:v>0.394213267</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.2176744</c:v>
+                  <c:v>0.39511625</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.2193033</c:v>
+                  <c:v>0.396202183</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.2205327</c:v>
+                  <c:v>0.397021767</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.2216362</c:v>
+                  <c:v>0.397757467</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.2231172</c:v>
+                  <c:v>0.3987448</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.2241165</c:v>
+                  <c:v>0.399411</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.225335</c:v>
+                  <c:v>0.400223367</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.2266658</c:v>
+                  <c:v>0.401110517</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.2275702</c:v>
+                  <c:v>0.401713433</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.2287094</c:v>
+                  <c:v>0.402472917</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.2298355</c:v>
+                  <c:v>0.403223633</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.2311755</c:v>
+                  <c:v>0.404117017</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.2319762</c:v>
+                  <c:v>0.4046508</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.2328864</c:v>
+                  <c:v>0.405257583</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.2337869</c:v>
+                  <c:v>0.4058579</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.2349038</c:v>
+                  <c:v>0.406602517</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.2357897</c:v>
+                  <c:v>0.407193133</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.2365741</c:v>
+                  <c:v>0.4077161</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.2375997</c:v>
+                  <c:v>0.408399783</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.2386189</c:v>
+                  <c:v>0.409079267</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.2392357</c:v>
+                  <c:v>0.40949045</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.2401806</c:v>
+                  <c:v>0.410120417</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.2411757</c:v>
+                  <c:v>0.4107838</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.2417002</c:v>
+                  <c:v>0.41113345</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.2425458</c:v>
+                  <c:v>0.411697217</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.2435277</c:v>
+                  <c:v>0.412351817</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.2441413</c:v>
+                  <c:v>0.412760867</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.2448565</c:v>
+                  <c:v>0.413237683</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.2457715</c:v>
+                  <c:v>0.413847667</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.2463712</c:v>
+                  <c:v>0.414247467</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.2470741</c:v>
+                  <c:v>0.4147161</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.2478112</c:v>
+                  <c:v>0.415207433</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.2484636</c:v>
+                  <c:v>0.415642417</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.2492716</c:v>
+                  <c:v>0.41618105</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.2497746</c:v>
+                  <c:v>0.416516383</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.2505009</c:v>
+                  <c:v>0.417000567</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.2512856</c:v>
+                  <c:v>0.417523733</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.2518579</c:v>
+                  <c:v>0.417905283</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.2523977</c:v>
+                  <c:v>0.41826515</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.2531656</c:v>
+                  <c:v>0.418777083</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.2536658</c:v>
+                  <c:v>0.41911055</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.2542638</c:v>
+                  <c:v>0.419509183</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.2549848</c:v>
+                  <c:v>0.41998985</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.255469</c:v>
+                  <c:v>0.42031265</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.2560577</c:v>
+                  <c:v>0.42070515</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.2566626</c:v>
+                  <c:v>0.421108417</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.2571829</c:v>
+                  <c:v>0.421455283</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.257855</c:v>
+                  <c:v>0.421903333</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.2582856</c:v>
+                  <c:v>0.4221904</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.2588711</c:v>
+                  <c:v>0.422580733</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.2595174</c:v>
+                  <c:v>0.423011617</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.2600086</c:v>
+                  <c:v>0.42333905</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.2604607</c:v>
+                  <c:v>0.42364045</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.2610858</c:v>
+                  <c:v>0.424057217</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.2615094</c:v>
+                  <c:v>0.424339633</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.2620292</c:v>
+                  <c:v>0.424686133</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.2626195</c:v>
+                  <c:v>0.42507965</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.2630242</c:v>
+                  <c:v>0.425349467</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.2635346</c:v>
+                  <c:v>0.425689717</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.2640497</c:v>
+                  <c:v>0.42603315</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.2644784</c:v>
+                  <c:v>0.42631895</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.2650551</c:v>
+                  <c:v>0.4267034</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.2654358</c:v>
+                  <c:v>0.426957183</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.2659232</c:v>
+                  <c:v>0.427282167</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.266471</c:v>
+                  <c:v>0.427647317</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.2669046</c:v>
+                  <c:v>0.4279364</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.2672952</c:v>
+                  <c:v>0.428196833</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.2678181</c:v>
+                  <c:v>0.428545433</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.2681862</c:v>
+                  <c:v>0.428790767</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.2686502</c:v>
+                  <c:v>0.429100133</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.2691465</c:v>
+                  <c:v>0.429431017</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.2694922</c:v>
+                  <c:v>0.4296615</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2112,11 +2216,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="338793712"/>
-        <c:axId val="338791392"/>
+        <c:axId val="956582592"/>
+        <c:axId val="956583952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="338793712"/>
+        <c:axId val="956582592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2172,12 +2276,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338791392"/>
+        <c:crossAx val="956583952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="338791392"/>
+        <c:axId val="956583952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2234,7 +2338,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338793712"/>
+        <c:crossAx val="956582592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3466,15 +3570,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>201971</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>540637</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>348226</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>619159</xdr:colOff>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>43016</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3515,21 +3619,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J101" totalsRowShown="0">
-  <autoFilter ref="A1:J101"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K101" totalsRowShown="0">
+  <autoFilter ref="A1:K101"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="W"/>
     <tableColumn id="2" name="T"/>
     <tableColumn id="3" name="X (energy b)"/>
     <tableColumn id="4" name="CA0"/>
-    <tableColumn id="5" name="Hrx" dataDxfId="1"/>
+    <tableColumn id="5" name="Hrx" dataDxfId="2"/>
     <tableColumn id="6" name="FA0"/>
     <tableColumn id="7" name="thetaCp"/>
     <tableColumn id="8" name="K"/>
-    <tableColumn id="9" name="ra" dataDxfId="0"/>
+    <tableColumn id="9" name="ra" dataDxfId="1"/>
     <tableColumn id="10" name="X(mass b)">
       <calculatedColumnFormula>H2/(1+H2)</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="11" name="X(eb)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3848,7 +3953,7 @@
         <v>12630297.721543629</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D54" si="1">C3/(1+C3)</f>
+        <f t="shared" ref="D3:D45" si="1">C3/(1+C3)</f>
         <v>0.99999992082530886</v>
       </c>
     </row>
@@ -4743,10 +4848,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" zoomScale="75" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4755,7 +4860,7 @@
     <col min="10" max="10" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4786,8 +4891,11 @@
       <c r="J1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4819,8 +4927,11 @@
         <f>H2/(1+H2)</f>
         <v>0.50401696658760686</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>11.639589000000001</v>
       </c>
@@ -4852,8 +4963,11 @@
         <f t="shared" ref="J3:J67" si="0">H3/(1+H3)</f>
         <v>3.7639460477584895E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>15.997234000000001</v>
       </c>
@@ -4885,8 +4999,11 @@
         <f t="shared" si="0"/>
         <v>2.9003660656199325E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20.237628999999998</v>
       </c>
@@ -4918,8 +5035,11 @@
         <f t="shared" si="0"/>
         <v>2.3866941350509371E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>26.472071</v>
       </c>
@@ -4951,8 +5071,11 @@
         <f t="shared" si="0"/>
         <v>1.9075258704186648E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>30.492588999999999</v>
       </c>
@@ -4984,8 +5107,11 @@
         <f t="shared" si="0"/>
         <v>1.6944823767207032E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>35.287385</v>
       </c>
@@ -5017,8 +5143,11 @@
         <f t="shared" si="0"/>
         <v>1.4990077995055643E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>41.397410000000001</v>
       </c>
@@ -5050,8 +5179,11 @@
         <f t="shared" si="0"/>
         <v>1.3106439924581595E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>45.502315000000003</v>
       </c>
@@ -5083,8 +5215,11 @@
         <f t="shared" si="0"/>
         <v>1.2103802995321027E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>50.444071999999998</v>
       </c>
@@ -5116,8 +5251,11 @@
         <f t="shared" si="0"/>
         <v>1.1096975291763476E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>55.665008</v>
       </c>
@@ -5149,8 +5287,11 @@
         <f t="shared" si="0"/>
         <v>1.0213115962936441E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>60.308922000000003</v>
       </c>
@@ -5182,8 +5323,11 @@
         <f t="shared" si="0"/>
         <v>9.5459956935059903E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>66.236969000000002</v>
       </c>
@@ -5215,8 +5359,11 @@
         <f t="shared" si="0"/>
         <v>8.8204080706203569E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>70.016673999999995</v>
       </c>
@@ -5248,8 +5395,11 @@
         <f t="shared" si="0"/>
         <v>8.4171501789906209E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>75.428263000000001</v>
       </c>
@@ -5281,8 +5431,11 @@
         <f t="shared" si="0"/>
         <v>7.9049144322949176E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="2">
+        <v>0.33121591700000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>81.415805000000006</v>
       </c>
@@ -5314,8 +5467,11 @@
         <f t="shared" si="0"/>
         <v>7.4116571560160285E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="2">
+        <v>0.3796619</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>85.910286999999997</v>
       </c>
@@ -5347,8 +5503,11 @@
         <f t="shared" si="0"/>
         <v>7.0833679613008767E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="2">
+        <v>0.38107693300000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>90.161195000000006</v>
       </c>
@@ -5380,8 +5539,11 @@
         <f t="shared" si="0"/>
         <v>6.8007333386105318E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="2">
+        <v>0.38235213299999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>96.232900999999998</v>
       </c>
@@ -5413,8 +5575,11 @@
         <f t="shared" si="0"/>
         <v>6.4370953466680071E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="2">
+        <v>0.38407806700000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>100.29774</v>
       </c>
@@ -5446,8 +5611,11 @@
         <f t="shared" si="0"/>
         <v>6.216513223183698E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="2">
+        <v>0.385176717</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>105.25851</v>
       </c>
@@ -5479,8 +5647,11 @@
         <f t="shared" si="0"/>
         <v>5.9685623641407542E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="2">
+        <v>0.38646171699999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>111.19604</v>
       </c>
@@ -5512,8 +5683,11 @@
         <f t="shared" si="0"/>
         <v>5.6988371150749478E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="2">
+        <v>0.38792624999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>115.26495</v>
       </c>
@@ -5545,8 +5719,11 @@
         <f t="shared" si="0"/>
         <v>5.5288617402688015E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="2">
+        <v>0.38888763300000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>120.33373</v>
       </c>
@@ -5578,8 +5755,11 @@
         <f t="shared" si="0"/>
         <v>5.3320171886584774E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="2">
+        <v>0.390041217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>125.57252</v>
       </c>
@@ -5611,8 +5791,11 @@
         <f t="shared" si="0"/>
         <v>5.1440024210815559E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="2">
+        <v>0.39118599999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>130.08080000000001</v>
       </c>
@@ -5644,8 +5827,11 @@
         <f t="shared" si="0"/>
         <v>4.9934404192559642E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="2">
+        <v>0.39213545</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>136.06339</v>
       </c>
@@ -5677,8 +5863,11 @@
         <f t="shared" si="0"/>
         <v>4.8079717269925541E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="2">
+        <v>0.39334826699999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>140.48876000000001</v>
       </c>
@@ -5710,8 +5899,11 @@
         <f t="shared" si="0"/>
         <v>4.6801927974279341E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="2">
+        <v>0.39421326699999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>145.25403</v>
       </c>
@@ -5743,8 +5935,11 @@
         <f t="shared" si="0"/>
         <v>4.5505973990499831E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30" s="2">
+        <v>0.39511625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>151.18805</v>
       </c>
@@ -5776,8 +5971,11 @@
         <f t="shared" si="0"/>
         <v>4.3998557176270908E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31" s="2">
+        <v>0.39620218299999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>155.81832</v>
       </c>
@@ -5809,8 +6007,11 @@
         <f t="shared" si="0"/>
         <v>4.2896198885581027E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="2">
+        <v>0.39702176700000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>160.08905999999999</v>
       </c>
@@ -5842,8 +6043,11 @@
         <f t="shared" si="0"/>
         <v>4.1931435113026069E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="2">
+        <v>0.39775746699999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>165.99534</v>
       </c>
@@ -5875,8 +6079,11 @@
         <f t="shared" si="0"/>
         <v>4.0672895960188185E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="2">
+        <v>0.39874480000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>170.09696</v>
       </c>
@@ -5908,8 +6115,11 @@
         <f t="shared" si="0"/>
         <v>3.9847581779574462E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35" s="2">
+        <v>0.39941100000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>175.22862000000001</v>
       </c>
@@ -5941,8 +6151,11 @@
         <f t="shared" si="0"/>
         <v>3.886436678654561E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36" s="2">
+        <v>0.400223367</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>181.00058000000001</v>
       </c>
@@ -5974,8 +6187,11 @@
         <f t="shared" si="0"/>
         <v>3.7819426112648546E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37" s="2">
+        <v>0.401110517</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>185.02591000000001</v>
       </c>
@@ -6007,8 +6223,11 @@
         <f t="shared" si="0"/>
         <v>3.7127640136268183E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38" s="2">
+        <v>0.40171343300000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>190.21749</v>
       </c>
@@ -6040,8 +6259,11 @@
         <f t="shared" si="0"/>
         <v>3.6273941090067502E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39" s="2">
+        <v>0.40247291699999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>195.48507000000001</v>
       </c>
@@ -6073,8 +6295,11 @@
         <f t="shared" si="0"/>
         <v>3.5450876416971339E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40" s="2">
+        <v>0.40322363300000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>201.93421000000001</v>
       </c>
@@ -6106,8 +6331,11 @@
         <f t="shared" si="0"/>
         <v>3.4498572840540617E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41" s="2">
+        <v>0.40411701700000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>205.88332</v>
       </c>
@@ -6139,8 +6367,11 @@
         <f t="shared" si="0"/>
         <v>3.3941405754422159E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42" s="2">
+        <v>0.40465079999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>210.46176</v>
       </c>
@@ -6172,8 +6403,11 @@
         <f>H43/(1+H43)</f>
         <v>3.3320602561516342E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43" s="2">
+        <v>0.40525758299999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>215.08636999999999</v>
       </c>
@@ -6205,8 +6439,11 @@
         <f t="shared" si="0"/>
         <v>3.2718597930433565E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44" s="2">
+        <v>0.40585789999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>220.95681999999999</v>
       </c>
@@ -6238,8 +6475,11 @@
         <f t="shared" si="0"/>
         <v>3.198735258555296E-3</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45" s="2">
+        <v>0.406602517</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>225.72111000000001</v>
       </c>
@@ -6271,8 +6511,11 @@
         <f t="shared" si="0"/>
         <v>3.1419967404737012E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46" s="2">
+        <v>0.40719313299999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>230.02101999999999</v>
       </c>
@@ -6304,8 +6547,11 @@
         <f t="shared" si="0"/>
         <v>3.0927054997281936E-3</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47" s="2">
+        <v>0.40771610000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>235.75996000000001</v>
       </c>
@@ -6337,8 +6583,11 @@
         <f t="shared" si="0"/>
         <v>3.029394880715458E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48" s="2">
+        <v>0.40839978300000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>241.59823</v>
       </c>
@@ -6370,8 +6619,11 @@
         <f t="shared" si="0"/>
         <v>2.9679649619014123E-3</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49" s="2">
+        <v>0.40907926700000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>245.19755000000001</v>
       </c>
@@ -6403,8 +6655,11 @@
         <f t="shared" si="0"/>
         <v>2.9313817376911879E-3</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50" s="2">
+        <v>0.40949045000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>250.81126</v>
       </c>
@@ -6436,8 +6691,11 @@
         <f t="shared" si="0"/>
         <v>2.8763030163191259E-3</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51" s="2">
+        <v>0.41012041700000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>256.85453999999999</v>
       </c>
@@ -6469,8 +6727,11 @@
         <f t="shared" si="0"/>
         <v>2.8195277851873831E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52" s="2">
+        <v>0.41078379999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>260.09519</v>
       </c>
@@ -6502,8 +6763,11 @@
         <f t="shared" si="0"/>
         <v>2.789994154354946E-3</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K53" s="2">
+        <v>0.41113345000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>265.40246000000002</v>
       </c>
@@ -6535,8 +6799,11 @@
         <f t="shared" si="0"/>
         <v>2.7432538572893682E-3</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K54" s="2">
+        <v>0.411697217</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>271.69378999999998</v>
       </c>
@@ -6568,8 +6835,11 @@
         <f t="shared" si="0"/>
         <v>2.6899446812058514E-3</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K55" s="2">
+        <v>0.41235181700000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>275.69684999999998</v>
       </c>
@@ -6601,8 +6871,11 @@
         <f t="shared" si="0"/>
         <v>2.6571208985022104E-3</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K56" s="2">
+        <v>0.41276086699999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>280.43405000000001</v>
       </c>
@@ -6634,8 +6907,11 @@
         <f t="shared" si="0"/>
         <v>2.6195200924292437E-3</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K57" s="2">
+        <v>0.41323768300000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>286.60683</v>
       </c>
@@ -6667,8 +6943,11 @@
         <f t="shared" si="0"/>
         <v>2.5722663822268749E-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K58" s="2">
+        <v>0.41384766699999997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>290.72260999999997</v>
       </c>
@@ -6700,8 +6979,11 @@
         <f t="shared" si="0"/>
         <v>2.5417231809902012E-3</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K59" s="2">
+        <v>0.41424746699999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>295.61846000000003</v>
       </c>
@@ -6733,8 +7015,11 @@
         <f t="shared" si="0"/>
         <v>2.5064021632843153E-3</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K60" s="2">
+        <v>0.41471609999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>300.83569999999997</v>
       </c>
@@ -6766,8 +7051,11 @@
         <f t="shared" si="0"/>
         <v>2.4699840724382361E-3</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K61" s="2">
+        <v>0.41520743300000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>305.52730000000003</v>
       </c>
@@ -6799,8 +7087,11 @@
         <f t="shared" si="0"/>
         <v>2.4382404526855461E-3</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K62" s="2">
+        <v>0.41564241699999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>311.43358000000001</v>
       </c>
@@ -6832,8 +7123,11 @@
         <f t="shared" si="0"/>
         <v>2.3995284143050722E-3</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K63" s="2">
+        <v>0.41618105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>315.16514999999998</v>
       </c>
@@ -6865,8 +7159,11 @@
         <f t="shared" si="0"/>
         <v>2.3757424070318944E-3</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K64" s="2">
+        <v>0.41651638299999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>320.62824999999998</v>
       </c>
@@ -6898,8 +7195,11 @@
         <f t="shared" si="0"/>
         <v>2.3418030856171309E-3</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K65" s="2">
+        <v>0.41700056699999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>326.63227000000001</v>
       </c>
@@ -6931,8 +7231,11 @@
         <f>H66/(1+H66)</f>
         <v>2.3057711323360582E-3</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K66" s="2">
+        <v>0.41752373300000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>331.07832999999999</v>
       </c>
@@ -6964,8 +7267,11 @@
         <f t="shared" si="0"/>
         <v>2.2798902228517615E-3</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K67" s="2">
+        <v>0.41790528300000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>335.32443999999998</v>
       </c>
@@ -6994,11 +7300,14 @@
         <v>-1.2635999999999999E-3</v>
       </c>
       <c r="J68">
-        <f t="shared" ref="J68:J107" si="1">H68/(1+H68)</f>
+        <f t="shared" ref="J68:J101" si="1">H68/(1+H68)</f>
         <v>2.255799862091797E-3</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K68" s="2">
+        <v>0.41826514999999997</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>341.45418999999998</v>
       </c>
@@ -7030,8 +7339,11 @@
         <f t="shared" si="1"/>
         <v>2.2218523791221706E-3</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K69" s="2">
+        <v>0.41877708299999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>345.50416999999999</v>
       </c>
@@ -7063,8 +7375,11 @@
         <f t="shared" si="1"/>
         <v>2.2000491117135828E-3</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K70" s="2">
+        <v>0.41911055000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>350.40550999999999</v>
       </c>
@@ -7096,8 +7411,11 @@
         <f t="shared" si="1"/>
         <v>2.1743618480968121E-3</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K71" s="2">
+        <v>0.41950918300000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>356.40341999999998</v>
       </c>
@@ -7129,8 +7447,11 @@
         <f t="shared" si="1"/>
         <v>2.1437942723852074E-3</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K72" s="2">
+        <v>0.41998985</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>360.48597999999998</v>
       </c>
@@ -7162,8 +7483,11 @@
         <f t="shared" si="1"/>
         <v>2.1234812319384355E-3</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K73" s="2">
+        <v>0.42031265000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>365.51017000000002</v>
       </c>
@@ -7195,8 +7519,11 @@
         <f t="shared" si="1"/>
         <v>2.0990845755952353E-3</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K74" s="2">
+        <v>0.42070515000000003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>370.74137000000002</v>
       </c>
@@ -7228,8 +7555,11 @@
         <f t="shared" si="1"/>
         <v>2.0742883841646754E-3</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K75" s="2">
+        <v>0.42110841700000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>375.29790000000003</v>
       </c>
@@ -7261,8 +7591,11 @@
         <f t="shared" si="1"/>
         <v>2.053275385893524E-3</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K76" s="2">
+        <v>0.42145528300000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>381.26233000000002</v>
       </c>
@@ -7294,8 +7627,11 @@
         <f t="shared" si="1"/>
         <v>2.0263854243957645E-3</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K77" s="2">
+        <v>0.42190333299999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>385.13128999999998</v>
       </c>
@@ -7327,8 +7663,11 @@
         <f t="shared" si="1"/>
         <v>2.0094539644425953E-3</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K78" s="2">
+        <v>0.42219040000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>390.45170000000002</v>
       </c>
@@ -7360,8 +7699,11 @@
         <f t="shared" si="1"/>
         <v>1.9865457806236687E-3</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K79" s="2">
+        <v>0.42258073299999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>396.40588000000002</v>
       </c>
@@ -7393,8 +7735,11 @@
         <f t="shared" si="1"/>
         <v>1.9616443879554731E-3</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K80" s="2">
+        <v>0.42301161700000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>400.98815999999999</v>
       </c>
@@ -7426,8 +7771,11 @@
         <f t="shared" si="1"/>
         <v>1.9429177220704455E-3</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K81" s="2">
+        <v>0.42333904999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>405.25081</v>
       </c>
@@ -7459,8 +7807,11 @@
         <f t="shared" si="1"/>
         <v>1.9258838145913646E-3</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K82" s="2">
+        <v>0.42364045</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>411.21600000000001</v>
       </c>
@@ -7492,8 +7843,11 @@
         <f t="shared" si="1"/>
         <v>1.9025733147474283E-3</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K83" s="2">
+        <v>0.42405721699999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>415.30545999999998</v>
       </c>
@@ -7525,8 +7879,11 @@
         <f t="shared" si="1"/>
         <v>1.8869327536292638E-3</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K84" s="2">
+        <v>0.42433963299999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>420.37599</v>
       </c>
@@ -7558,8 +7915,11 @@
         <f t="shared" si="1"/>
         <v>1.8679044036989179E-3</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K85" s="2">
+        <v>0.42468613300000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>426.20584000000002</v>
       </c>
@@ -7591,8 +7951,11 @@
         <f t="shared" si="1"/>
         <v>1.8465838199331239E-3</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K86" s="2">
+        <v>0.42507964999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>430.24747000000002</v>
       </c>
@@ -7624,8 +7987,11 @@
         <f t="shared" si="1"/>
         <v>1.8321371123303173E-3</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K87" s="2">
+        <v>0.42534946699999998</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>435.39604000000003</v>
       </c>
@@ -7657,8 +8023,11 @@
         <f t="shared" si="1"/>
         <v>1.814103049118532E-3</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K88" s="2">
+        <v>0.42568971700000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>440.65215999999998</v>
       </c>
@@ -7690,8 +8059,11 @@
         <f t="shared" si="1"/>
         <v>1.7959686931273253E-3</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K89" s="2">
+        <v>0.42603315000000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>445.07225</v>
       </c>
@@ -7723,8 +8095,11 @@
         <f t="shared" si="1"/>
         <v>1.7811219441151154E-3</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K90" s="2">
+        <v>0.42631894999999997</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>451.08454999999998</v>
       </c>
@@ -7756,8 +8131,11 @@
         <f t="shared" si="1"/>
         <v>1.7612923757322578E-3</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K91" s="2">
+        <v>0.42670340000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>455.09579000000002</v>
       </c>
@@ -7789,8 +8167,11 @@
         <f t="shared" si="1"/>
         <v>1.748437611523417E-3</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K92" s="2">
+        <v>0.42695718300000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>460.2817</v>
       </c>
@@ -7822,8 +8203,11 @@
         <f t="shared" si="1"/>
         <v>1.7319949886946148E-3</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K93" s="2">
+        <v>0.42728216699999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>466.17581999999999</v>
       </c>
@@ -7855,8 +8239,11 @@
         <f t="shared" si="1"/>
         <v>1.7137579916557245E-3</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K94" s="2">
+        <v>0.42764731700000003</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>470.89283999999998</v>
       </c>
@@ -7888,8 +8275,11 @@
         <f t="shared" si="1"/>
         <v>1.6994070992948701E-3</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K95" s="2">
+        <v>0.42793639999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>475.18133999999998</v>
       </c>
@@ -7921,8 +8311,11 @@
         <f t="shared" si="1"/>
         <v>1.686650404142202E-3</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K96" s="2">
+        <v>0.428196833</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>480.97978000000001</v>
       </c>
@@ -7954,8 +8347,11 @@
         <f t="shared" si="1"/>
         <v>1.6697074143495005E-3</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K97" s="2">
+        <v>0.42854543299999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>485.10097999999999</v>
       </c>
@@ -7987,8 +8383,11 @@
         <f t="shared" si="1"/>
         <v>1.6578469793061643E-3</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K98" s="2">
+        <v>0.42879076700000002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>490.34536000000003</v>
       </c>
@@ -8020,8 +8419,11 @@
         <f t="shared" si="1"/>
         <v>1.6430957929439729E-3</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K99" s="2">
+        <v>0.42910013299999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>496.01432</v>
       </c>
@@ -8053,8 +8455,11 @@
         <f t="shared" si="1"/>
         <v>1.6274470984847598E-3</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K100" s="2">
+        <v>0.42943101700000003</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>500</v>
       </c>
@@ -8085,6 +8490,9 @@
       <c r="J101">
         <f t="shared" si="1"/>
         <v>1.6166821066646779E-3</v>
+      </c>
+      <c r="K101" s="2">
+        <v>0.42966149999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>